<commit_message>
proyecto carrito de la compra
</commit_message>
<xml_diff>
--- a/lvh_xoias/Presupuesto.xlsx
+++ b/lvh_xoias/Presupuesto.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programación\PROYECTOS\lvh_xoias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{BAE93593-A9F1-454F-815F-27AEF9690B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED267B6B-F243-4DEB-AC41-9A0777E3698F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="35160" yWindow="1500" windowWidth="19395" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="lvhXoias" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,9 +45,6 @@
     <t>Módulo SEO</t>
   </si>
   <si>
-    <t>Desarrollo, Diseño web, curso de implantación</t>
-  </si>
-  <si>
     <t>PAGO ÚNICO</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
     <t>Pasarela de pago (0,2% sobre el PVP de cada producto)</t>
   </si>
   <si>
-    <t>1º Año:</t>
-  </si>
-  <si>
-    <t>otros años:</t>
-  </si>
-  <si>
     <t>MENSUAL</t>
   </si>
   <si>
@@ -82,16 +73,25 @@
   </si>
   <si>
     <t>Dominio (copra/renovación)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>A partir del segundo año:</t>
+  </si>
+  <si>
+    <t>Desarrollo, Diseño web, integración y curso de implantación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +99,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor theme="9" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,21 +137,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -141,6 +206,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F1D2F46-F5EB-4B0B-9D8A-35CA18A39C12}" name="Tabla1" displayName="Tabla1" ref="B5:F15" totalsRowCount="1" headerRowDxfId="4">
+  <autoFilter ref="B5:F14" xr:uid="{4F1D2F46-F5EB-4B0B-9D8A-35CA18A39C12}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2D4A4EDC-E193-43E0-8325-284E42A631AE}" name="CONCEPTO" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{82B0F519-DC6E-4FE9-9D8C-F24FD6DD99B4}" name="PAGO"/>
+    <tableColumn id="3" xr3:uid="{E08A0E62-9E67-4EBA-A003-4559D27D94A6}" name="PVP" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DEB4EB2F-CE30-4F4A-B34A-D0690ECB11A1}" name="IVA" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{4343E6FC-3273-4AD2-8888-F0923D71BCCB}" name="TOTAL (IVA Inc.)" totalsRowFunction="sum" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,23 +518,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -467,15 +549,15 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>19.989999999999998</v>
@@ -489,9 +571,9 @@
         <v>290.25479999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -508,9 +590,9 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -527,12 +609,12 @@
         <v>13.31</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>120</v>
@@ -545,13 +627,17 @@
         <f>IF(C9="MENSUAL",12*(D9+E9),D9+E9)</f>
         <v>145.19999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>30*1.21</f>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>70</v>
@@ -564,13 +650,17 @@
         <f t="shared" ref="F10:F13" si="1">IF(C10="MENSUAL",12*(D10+E10),D10+E10)</f>
         <v>84.7</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" ref="G10:G12" si="2">20*1.21</f>
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1">
         <v>200</v>
@@ -583,13 +673,17 @@
         <f t="shared" si="1"/>
         <v>242</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1">
         <v>70</v>
@@ -602,13 +696,17 @@
         <f t="shared" si="1"/>
         <v>84.7</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
       </c>
       <c r="D13" s="1">
         <v>1400</v>
@@ -622,35 +720,37 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
-        <f>SUM(F6:F14)</f>
+      <c r="F15" s="4">
+        <f>SUBTOTAL(109,Tabla1[TOTAL (IVA Inc.)])</f>
         <v>2578.3648000000003</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1">
-        <f>SUMIF(C6:C14,"&lt;&gt;PAGO ÚNICO",F6:F14)</f>
-        <v>327.76479999999998</v>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5">
+        <f>SUMIF(C6:C14,"&lt;&gt;PAGO ÚNICO",F6:F14)+SUM(G6:G14)</f>
+        <v>436.66480000000001</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
@@ -661,7 +761,6 @@
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
@@ -728,12 +827,20 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C14 C16:C35" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PAGO ÚNICO, MENSUAL, ANUAL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>